<commit_message>
Add patient name in patient excel
</commit_message>
<xml_diff>
--- a/utils/excel/export_patient_data.xlsx
+++ b/utils/excel/export_patient_data.xlsx
@@ -12,7 +12,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+  <si>
+    <t>Patient</t>
+  </si>
+  <si>
+    <t>Emeliza Yabut</t>
+  </si>
   <si>
     <t>Date</t>
   </si>
@@ -140,86 +146,94 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView showGridLines="1" workbookViewId="0" rightToLeft="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12">
-      <c r="A2" s="0" t="s">
+      <c r="K2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="L2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="0" t="s">
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="B3" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="C3" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="D3" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" s="0" t="s">
+      <c r="E3" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="F3" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="0" t="s">
+      <c r="G3" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="K2" s="0" t="s">
+      <c r="I3" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="L2" s="0" t="s">
+      <c r="J3" s="0" t="s">
         <v>22</v>
+      </c>
+      <c r="K3" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3" s="0" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -229,38 +243,38 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView showGridLines="1" workbookViewId="0" rightToLeft="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="0" t="s">
-        <v>17</v>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add delay to export
</commit_message>
<xml_diff>
--- a/utils/excel/export_patient_data.xlsx
+++ b/utils/excel/export_patient_data.xlsx
@@ -249,6 +249,14 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>2</v>

</xml_diff>